<commit_message>
yay! got visualizations for LWT and SNL sorted
</commit_message>
<xml_diff>
--- a/data/SNL-topics.xlsx
+++ b/data/SNL-topics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annafetter/Documents/political-satire/r-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E277829-5B82-1540-A684-D771A6171E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2434D53D-BBBE-044E-A813-3C029412A0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1056,14 +1056,15 @@
   </sheetPr>
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="319" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="71" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="48.1640625" customWidth="1"/>
     <col min="5" max="6" width="18.33203125" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" customWidth="1"/>
     <col min="8" max="8" width="15.5" customWidth="1"/>
@@ -1113,7 +1114,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11">
-        <v>45593</v>
+        <v>45563</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
@@ -1154,7 +1155,7 @@
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="11">
-        <v>45593</v>
+        <v>45563</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>24</v>

</xml_diff>